<commit_message>
Added scripts and project sections
</commit_message>
<xml_diff>
--- a/processing/final/benchmark_clients/benchmark_clients.xlsx
+++ b/processing/final/benchmark_clients/benchmark_clients.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37420" yWindow="440" windowWidth="35420" windowHeight="19800" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="440" windowWidth="35420" windowHeight="19800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -233,8 +233,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -252,7 +252,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -342,7 +354,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -404,8 +416,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$E$5:$E$13</c:f>
               <c:numCache>
@@ -440,7 +452,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -459,7 +471,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -549,7 +573,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -611,8 +635,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$E$14:$E$22</c:f>
               <c:numCache>
@@ -647,7 +671,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -658,12 +682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="985503632"/>
-        <c:axId val="985507760"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="985503632"/>
+        <c:axId val="-1230867248"/>
+        <c:axId val="-1278208160"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1230867248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,15 +792,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="985507760"/>
+        <c:crossAx val="-1278208160"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="985507760"/>
+        <c:axId val="-1278208160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,9 +915,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="985503632"/>
+        <c:crossAx val="-1230867248"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1055,8 +1075,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1074,7 +1094,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -1164,7 +1196,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -1226,8 +1258,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$G$5:$G$13</c:f>
               <c:numCache>
@@ -1262,7 +1294,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -1281,7 +1313,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -1371,7 +1415,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -1433,8 +1477,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$G$14:$G$22</c:f>
               <c:numCache>
@@ -1469,7 +1513,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -1480,12 +1524,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="485995360"/>
-        <c:axId val="486502032"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="485995360"/>
+        <c:axId val="-1232766688"/>
+        <c:axId val="-1437726048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1232766688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,15 +1634,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="486502032"/>
+        <c:crossAx val="-1437726048"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="486502032"/>
+        <c:axId val="-1437726048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,9 +1752,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="485995360"/>
+        <c:crossAx val="-1232766688"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3741,8 +3781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added sections in report
</commit_message>
<xml_diff>
--- a/processing/final/benchmark_clients/benchmark_clients.xlsx
+++ b/processing/final/benchmark_clients/benchmark_clients.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="440" windowWidth="35420" windowHeight="19800" tabRatio="500"/>
+    <workbookView xWindow="-37440" yWindow="440" windowWidth="35420" windowHeight="19800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>BENCHMARK_CLIENTS</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Total clients</t>
+  </si>
+  <si>
+    <t>Latency from Interactive law</t>
+  </si>
+  <si>
+    <t>Identity Function</t>
   </si>
 </sst>
 </file>
@@ -356,63 +365,36 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$D$5:$D$22</c:f>
+              <c:f>data!$D$26:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.0</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48.0</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>56.0</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,63 +557,36 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$D$5:$D$22</c:f>
+              <c:f>data!$D$26:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.0</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48.0</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>56.0</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,11 +637,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1230867248"/>
-        <c:axId val="-1278208160"/>
+        <c:axId val="-327742656"/>
+        <c:axId val="-327739264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1230867248"/>
+        <c:axId val="-327742656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -713,7 +668,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of clients per thread</a:t>
+                  <a:t>Total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> n</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>umber of clients</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -722,8 +685,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.358827109801459"/>
-              <c:y val="0.844436901805658"/>
+              <c:x val="0.383697605156868"/>
+              <c:y val="0.877300839155669"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -792,12 +755,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1278208160"/>
+        <c:crossAx val="-327739264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1278208160"/>
+        <c:axId val="-327739264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -915,7 +878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1230867248"/>
+        <c:crossAx val="-327742656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1198,63 +1161,36 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$D$5:$D$22</c:f>
+              <c:f>data!$D$26:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.0</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48.0</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>56.0</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1417,63 +1353,36 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$D$5:$D$22</c:f>
+              <c:f>data!$D$26:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.0</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.0</c:v>
+                  <c:v>80.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48.0</c:v>
+                  <c:v>96.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>56.0</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1524,11 +1433,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1232766688"/>
-        <c:axId val="-1437726048"/>
+        <c:axId val="-327807744"/>
+        <c:axId val="-327804352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1232766688"/>
+        <c:axId val="-327807744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,7 +1464,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of clients per thread</a:t>
+                  <a:t>Total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> n</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>umber of clients</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1564,8 +1481,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.358827109801459"/>
-              <c:y val="0.844436901805658"/>
+              <c:x val="0.425011196247832"/>
+              <c:y val="0.877300839155669"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1634,12 +1551,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1437726048"/>
+        <c:crossAx val="-327804352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1437726048"/>
+        <c:axId val="-327804352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,7 +1669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1232766688"/>
+        <c:crossAx val="-327807744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1767,6 +1684,662 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Interactive Law</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Read</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$F$26:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.231944316116911</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.486246415011089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.939073698434653</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.374142619198653</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.738433269116892</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.366241116218613</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.966453717682698</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.647806604436924</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.262310929749324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$G$5:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.8040625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.98304166667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.30022916667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.628</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.93047916667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.46041666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.002875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6698125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.26677083333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Write</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$F$35:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.230355957356652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.481259749698876</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.918915812565133</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.28611367521103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.568936473679774</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.107200228513712</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.68712657041346</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.377640668288462</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.030506804853436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$G$14:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.7905</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.95739583333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.28139583333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.57002083333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.82491666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.28170833333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8245625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.49329166667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.16939583333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Identity function</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="70AD47"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$I$26:$I$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$I$26:$I$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="90976848"/>
+        <c:axId val="122967248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="90976848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> from interactive law (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.383697605156868"/>
+              <c:y val="0.877300839155669"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="122967248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="122967248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Latency measured</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> by clients (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0220858895705521"/>
+              <c:y val="0.302870833697293"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90976848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1913,6 +2486,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2945,20 +3558,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2979,16 +4108,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3004,6 +4133,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3777,12 +4938,264 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5141,6 +6554,224 @@
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f>D14*2</f>
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F26">
+        <f>D26/E5*1000</f>
+        <v>1.2319443161169115</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f t="shared" ref="D27:D34" si="0">D15*2</f>
+        <v>8</v>
+      </c>
+      <c r="E27" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F34" si="1">D27/E6*1000</f>
+        <v>1.4862464150110888</v>
+      </c>
+      <c r="I27">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E28" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1.9390736984346526</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>2.3741426191986528</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E30" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>2.7384332691168924</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>3.366241116218613</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>3.9664537176826982</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E33" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>4.6478066044369237</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="E34" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>5.262310929749324</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E35" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F35">
+        <f>D26/E14*1000</f>
+        <v>1.2303559573566516</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E36" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:F43" si="2">D27/E15*1000</f>
+        <v>1.481259749698876</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E37" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>1.9189158125651331</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E38" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>2.2861136752110296</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E39" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>2.568936473679774</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E40" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>3.1072002285137121</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E41" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>3.6871265704134597</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E42" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>4.3776406682884623</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E43" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>5.0305068048534363</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>